<commit_message>
Swing-exportfunctionaliteit en configuratieondersteuning toevoegen
Introduceert tbl_MakeSwing.R als een skelet voor het exporteren van Swing-compatibele Excel-bestanden. Werkt tbl_maken.R bij om nieuwe Swing-configuratiebladen te lezen, ‘swing_output’-instellingen te verwerken en voorwaardelijk Swing-uitvoerbestanden te genereren. Werkt ook het configuratiebestand bij om deze wijzigingen te ondersteunen.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Github\GGData_tabellenboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1CC452C-7172-4EA0-8B53-CFDA74A2F23A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD19B13-99EB-41A9-8391-63DB80C53158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="8" activeTab="10" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -23,9 +23,10 @@
     <sheet name="indeling_rijen" sheetId="2" r:id="rId8"/>
     <sheet name="intro_tekst" sheetId="9" r:id="rId9"/>
     <sheet name="labelcorrectie" sheetId="7" r:id="rId10"/>
-    <sheet name="logos" sheetId="8" r:id="rId11"/>
-    <sheet name="onderdelen" sheetId="4" r:id="rId12"/>
-    <sheet name="opmaak" sheetId="6" r:id="rId13"/>
+    <sheet name="swing" sheetId="14" r:id="rId11"/>
+    <sheet name="logos" sheetId="8" r:id="rId12"/>
+    <sheet name="onderdelen" sheetId="4" r:id="rId13"/>
+    <sheet name="opmaak" sheetId="6" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="186">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -561,6 +562,51 @@
   </si>
   <si>
     <t>BH</t>
+  </si>
+  <si>
+    <t>swing_output</t>
+  </si>
+  <si>
+    <t>swing_output_bestandsnaam</t>
+  </si>
+  <si>
+    <t>kubusdata</t>
+  </si>
+  <si>
+    <t>inidcator_val</t>
+  </si>
+  <si>
+    <t>indicator_code</t>
+  </si>
+  <si>
+    <t>indicator_label</t>
+  </si>
+  <si>
+    <t>measure</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>decimals</t>
+  </si>
+  <si>
+    <t>include_crossing</t>
+  </si>
+  <si>
+    <t>SLAAPSLECHT</t>
+  </si>
+  <si>
+    <t>geo_subset</t>
+  </si>
+  <si>
+    <t>geo_code_source</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -923,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +989,7 @@
     <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -998,8 +1044,14 @@
       <c r="R1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1053,6 +1105,12 @@
       </c>
       <c r="R2" t="b">
         <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1133,6 +1191,70 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A35892-6DC7-4D7C-8E8A-C0994C6B6367}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1187,12 +1309,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,12 +1428,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,7 +1977,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Voeg kubusdata-exportfunctionaliteit toe voor Swing
Introduceert een nieuw script `tbl_MakeKubus.R` voor het genereren van platte kubusdata-exports die compatibel zijn met Swing (ABF), op basis van configuratie en variabele selectie. Werkt `tbl_maken.R` bij om deze nieuwe export te laden en aan te roepen wanneer `swing_output` is ingeschakeld, inclusief configuratievalidatie en integratie met de hoofdworkflow. Voegt ook het `glue`-pakket toe als afhankelijkheid en verwijdert de oude Swing-exportlogica.

Implement initial Swing export to Excel

Added logic to tbl_MakeSwing.R for creating and saving Excel workbooks with data and metadata sheets. Updated tbl_maken.R to adjust sheet loading and Swing export call, removing unused sheets and parameters. Updated configuratie.xlsx to reflect changes in configuration.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Github\GGData_tabellenboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD19B13-99EB-41A9-8391-63DB80C53158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39248C5C-D44F-4681-A09A-2B957D9E45CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="8" activeTab="10" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="10545" tabRatio="731" activeTab="2" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
-    <sheet name="algemeen" sheetId="5" r:id="rId1"/>
-    <sheet name="crossings" sheetId="3" r:id="rId2"/>
-    <sheet name="datasets" sheetId="1" r:id="rId3"/>
-    <sheet name="dichotoom" sheetId="11" r:id="rId4"/>
-    <sheet name="niet_dichotoom" sheetId="12" r:id="rId5"/>
-    <sheet name="forceer_datatypen" sheetId="13" r:id="rId6"/>
-    <sheet name="headers_afkortingen" sheetId="10" r:id="rId7"/>
-    <sheet name="indeling_rijen" sheetId="2" r:id="rId8"/>
-    <sheet name="intro_tekst" sheetId="9" r:id="rId9"/>
-    <sheet name="labelcorrectie" sheetId="7" r:id="rId10"/>
-    <sheet name="swing" sheetId="14" r:id="rId11"/>
-    <sheet name="logos" sheetId="8" r:id="rId12"/>
-    <sheet name="onderdelen" sheetId="4" r:id="rId13"/>
-    <sheet name="opmaak" sheetId="6" r:id="rId14"/>
+    <sheet name="swing_algemeen" sheetId="16" r:id="rId1"/>
+    <sheet name="swing_configuraties" sheetId="17" r:id="rId2"/>
+    <sheet name="algemeen" sheetId="5" r:id="rId3"/>
+    <sheet name="crossings" sheetId="3" r:id="rId4"/>
+    <sheet name="datasets" sheetId="1" r:id="rId5"/>
+    <sheet name="dichotoom" sheetId="11" r:id="rId6"/>
+    <sheet name="niet_dichotoom" sheetId="12" r:id="rId7"/>
+    <sheet name="forceer_datatypen" sheetId="13" r:id="rId8"/>
+    <sheet name="headers_afkortingen" sheetId="10" r:id="rId9"/>
+    <sheet name="indeling_rijen" sheetId="2" r:id="rId10"/>
+    <sheet name="intro_tekst" sheetId="9" r:id="rId11"/>
+    <sheet name="labelcorrectie" sheetId="7" r:id="rId12"/>
+    <sheet name="logos" sheetId="8" r:id="rId13"/>
+    <sheet name="onderdelen" sheetId="4" r:id="rId14"/>
+    <sheet name="opmaak" sheetId="6" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="215">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -573,40 +574,127 @@
     <t>kubusdata</t>
   </si>
   <si>
-    <t>inidcator_val</t>
-  </si>
-  <si>
-    <t>indicator_code</t>
-  </si>
-  <si>
-    <t>indicator_label</t>
-  </si>
-  <si>
-    <t>measure</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>decimals</t>
-  </si>
-  <si>
-    <t>include_crossing</t>
-  </si>
-  <si>
     <t>SLAAPSLECHT</t>
   </si>
   <si>
-    <t>geo_subset</t>
-  </si>
-  <si>
-    <t>geo_code_source</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>bron</t>
+  </si>
+  <si>
+    <t>meer_jaren_in_bestand</t>
+  </si>
+  <si>
+    <t>jaren_voor_analyse</t>
+  </si>
+  <si>
+    <t>type_periode</t>
+  </si>
+  <si>
+    <t>is_gewogen</t>
+  </si>
+  <si>
+    <t>gebiedsniveau</t>
+  </si>
+  <si>
+    <t>gebiedsindeling</t>
+  </si>
+  <si>
+    <t>minimum_observaties</t>
+  </si>
+  <si>
+    <t>geen_crossings</t>
+  </si>
+  <si>
+    <t>platte_kubus</t>
+  </si>
+  <si>
+    <t>T:/Projecten/Project E-MOVO/2023/3 Uitvoering/Data/Swing/GMJE 2023 - Analysebestand v7.0 Swing.sav</t>
+  </si>
+  <si>
+    <t>gmjeugd</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>Jaar</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>weegfactor_landelijk</t>
+  </si>
+  <si>
+    <t>ggd</t>
+  </si>
+  <si>
+    <t>Regiovar_met_uniekenaam</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>variabelen</t>
+  </si>
+  <si>
+    <t>MBOKA3S31</t>
+  </si>
+  <si>
+    <t>MBMRK3S1</t>
+  </si>
+  <si>
+    <t>EBEGK3S2</t>
+  </si>
+  <si>
+    <t>EBGLK3S1</t>
+  </si>
+  <si>
+    <t>PBMHK3S3</t>
+  </si>
+  <si>
+    <t>SBOSK3S2</t>
+  </si>
+  <si>
+    <t>SBOSK3S8</t>
+  </si>
+  <si>
+    <t>SBRLK3S11</t>
+  </si>
+  <si>
+    <t>LBRAK3S21</t>
+  </si>
+  <si>
+    <t>LBSDK3S1</t>
+  </si>
+  <si>
+    <t>SBSGK3S2</t>
+  </si>
+  <si>
+    <t>LFMGL1S2</t>
+  </si>
+  <si>
+    <t>PLAUK3S1</t>
+  </si>
+  <si>
+    <t>LLSIK3S1</t>
+  </si>
+  <si>
+    <t>LLSIK3S2</t>
+  </si>
+  <si>
+    <t>KLAS1</t>
+  </si>
+  <si>
+    <t>SBGMK3S2Q</t>
+  </si>
+  <si>
+    <t>SOOSK3S2</t>
+  </si>
+  <si>
+    <t>crossings</t>
   </si>
 </sst>
 </file>
@@ -968,149 +1056,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F3E72B-5A5D-4F06-93A4-3D37DD35ABC5}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>178</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>179</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>180</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="J1" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="K1" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="L1" t="s">
-        <v>61</v>
+        <v>184</v>
       </c>
       <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P1" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>130</v>
-      </c>
-      <c r="R1" t="s">
-        <v>163</v>
-      </c>
-      <c r="S1" t="s">
-        <v>171</v>
-      </c>
-      <c r="T1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>189</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
+        <v>175</v>
+      </c>
+      <c r="H2" t="s">
+        <v>191</v>
       </c>
       <c r="I2" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="J2" t="s">
-        <v>156</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0.05</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>150</v>
-      </c>
-      <c r="R2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>173</v>
+        <v>193</v>
+      </c>
+      <c r="K2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M2" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1119,6 +1156,327 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="5" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22162FB-19FC-4D35-A378-DB18D18AE0D2}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1190,71 +1548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A35892-6DC7-4D7C-8E8A-C0994C6B6367}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" t="s">
-        <v>184</v>
-      </c>
-      <c r="I2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1309,7 +1603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -1428,7 +1722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -1696,6 +1990,277 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7950D2-CBC9-4212-975C-6B7B88BFFA2B}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:T2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0.05</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FFED35-A9FD-48DB-B137-EE60E86B3C7B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1745,7 +2310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1838,7 +2403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B9AAB2-B21C-4F9A-AA85-AAC79B043700}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1858,7 +2423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BC63A0-66D1-48A8-8EE0-6CAC0789D923}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1878,7 +2443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C5E0E0-AEC7-4A98-8EDA-BFF72DE4F63D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1912,7 +2477,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7757E3CE-16FD-40F5-A230-112008D36DE8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1970,325 +2535,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="5" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update configuratie.xlsx voor werking met nieuwe functie swing platte kubus
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Github\GGData_tabellenboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39248C5C-D44F-4681-A09A-2B957D9E45CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17B1887-B183-4C10-96A4-B1DE6FF4E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="10545" tabRatio="731" activeTab="2" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="731" firstSheet="4" activeTab="13" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
-    <sheet name="swing_algemeen" sheetId="16" r:id="rId1"/>
-    <sheet name="swing_configuraties" sheetId="17" r:id="rId2"/>
-    <sheet name="algemeen" sheetId="5" r:id="rId3"/>
-    <sheet name="crossings" sheetId="3" r:id="rId4"/>
-    <sheet name="datasets" sheetId="1" r:id="rId5"/>
-    <sheet name="dichotoom" sheetId="11" r:id="rId6"/>
-    <sheet name="niet_dichotoom" sheetId="12" r:id="rId7"/>
-    <sheet name="forceer_datatypen" sheetId="13" r:id="rId8"/>
-    <sheet name="headers_afkortingen" sheetId="10" r:id="rId9"/>
-    <sheet name="indeling_rijen" sheetId="2" r:id="rId10"/>
-    <sheet name="intro_tekst" sheetId="9" r:id="rId11"/>
-    <sheet name="labelcorrectie" sheetId="7" r:id="rId12"/>
-    <sheet name="logos" sheetId="8" r:id="rId13"/>
-    <sheet name="onderdelen" sheetId="4" r:id="rId14"/>
-    <sheet name="opmaak" sheetId="6" r:id="rId15"/>
+    <sheet name="algemeen" sheetId="5" r:id="rId1"/>
+    <sheet name="crossings" sheetId="3" r:id="rId2"/>
+    <sheet name="datasets" sheetId="1" r:id="rId3"/>
+    <sheet name="dichotoom" sheetId="11" r:id="rId4"/>
+    <sheet name="niet_dichotoom" sheetId="12" r:id="rId5"/>
+    <sheet name="forceer_datatypen" sheetId="13" r:id="rId6"/>
+    <sheet name="headers_afkortingen" sheetId="10" r:id="rId7"/>
+    <sheet name="indeling_rijen" sheetId="2" r:id="rId8"/>
+    <sheet name="intro_tekst" sheetId="9" r:id="rId9"/>
+    <sheet name="labelcorrectie" sheetId="7" r:id="rId10"/>
+    <sheet name="logos" sheetId="8" r:id="rId11"/>
+    <sheet name="onderdelen" sheetId="4" r:id="rId12"/>
+    <sheet name="opmaak" sheetId="6" r:id="rId13"/>
+    <sheet name="swing_configuraties" sheetId="20" r:id="rId14"/>
+    <sheet name="swing_variabelen" sheetId="18" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="211">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -583,60 +583,24 @@
     <t>bron</t>
   </si>
   <si>
-    <t>meer_jaren_in_bestand</t>
-  </si>
-  <si>
-    <t>jaren_voor_analyse</t>
-  </si>
-  <si>
     <t>type_periode</t>
   </si>
   <si>
-    <t>is_gewogen</t>
-  </si>
-  <si>
     <t>gebiedsniveau</t>
   </si>
   <si>
-    <t>gebiedsindeling</t>
-  </si>
-  <si>
-    <t>minimum_observaties</t>
-  </si>
-  <si>
     <t>geen_crossings</t>
   </si>
   <si>
-    <t>platte_kubus</t>
-  </si>
-  <si>
-    <t>T:/Projecten/Project E-MOVO/2023/3 Uitvoering/Data/Swing/GMJE 2023 - Analysebestand v7.0 Swing.sav</t>
-  </si>
-  <si>
-    <t>gmjeugd</t>
-  </si>
-  <si>
     <t>FALSE</t>
   </si>
   <si>
     <t>Jaar</t>
   </si>
   <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>weegfactor_landelijk</t>
-  </si>
-  <si>
     <t>ggd</t>
   </si>
   <si>
-    <t>Regiovar_met_uniekenaam</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>variabelen</t>
   </si>
   <si>
@@ -695,19 +659,49 @@
   </si>
   <si>
     <t>crossings</t>
+  </si>
+  <si>
+    <t>gebiedsindeling_kolom</t>
+  </si>
+  <si>
+    <t>jaar_voor_analyse</t>
+  </si>
+  <si>
+    <t>Twente2024</t>
+  </si>
+  <si>
+    <t>gmjv</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>nederland</t>
+  </si>
+  <si>
+    <t>gemeente</t>
+  </si>
+  <si>
+    <t>gemeentecode_regio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -732,8 +726,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -744,8 +739,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="1" xr:uid="{53D9D93D-0541-4499-ACAE-C2999691F90B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1056,427 +1052,158 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F3E72B-5A5D-4F06-93A4-3D37DD35ABC5}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>181</v>
-      </c>
-      <c r="J1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L1" t="s">
-        <v>184</v>
-      </c>
-      <c r="M1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" t="s">
-        <v>189</v>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H2" t="s">
-        <v>191</v>
+        <v>65</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="J2" t="s">
-        <v>193</v>
-      </c>
-      <c r="K2" t="s">
-        <v>194</v>
-      </c>
-      <c r="L2" t="s">
-        <v>188</v>
-      </c>
-      <c r="M2" t="s">
-        <v>175</v>
+        <v>156</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0.05</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="5" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22162FB-19FC-4D35-A378-DB18D18AE0D2}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1548,7 +1275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1603,7 +1330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -1722,7 +1449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -1989,12 +1716,142 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7950D2-CBC9-4212-975C-6B7B88BFFA2B}">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3ECE10-9C11-42F2-BAC4-98A7CB15471E}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="I20:J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2">
+        <v>2024</v>
+      </c>
+      <c r="F2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3">
+        <v>2024</v>
+      </c>
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4">
+        <v>2024</v>
+      </c>
+      <c r="F4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E5">
+        <v>2024</v>
+      </c>
+      <c r="F5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE8AA37-4D9A-4ED0-A142-2CF818365C43}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,15 +1861,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
         <v>174</v>
@@ -2020,87 +1877,87 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2108,164 +1965,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P1" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>130</v>
-      </c>
-      <c r="R1" t="s">
-        <v>163</v>
-      </c>
-      <c r="S1" t="s">
-        <v>171</v>
-      </c>
-      <c r="T1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J2" t="s">
-        <v>156</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0.05</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>150</v>
-      </c>
-      <c r="R2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FFED35-A9FD-48DB-B137-EE60E86B3C7B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,12 +2015,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2403,7 +2108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B9AAB2-B21C-4F9A-AA85-AAC79B043700}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2423,7 +2128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BC63A0-66D1-48A8-8EE0-6CAC0789D923}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2443,7 +2148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C5E0E0-AEC7-4A98-8EDA-BFF72DE4F63D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2477,7 +2182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7757E3CE-16FD-40F5-A230-112008D36DE8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2535,4 +2240,325 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="5" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for swing_crossings in kubus data creation
Introduces the 'crossings' parameter to the MaakKubusData function and updates its handling to support data frames and missing values. Also ensures 'swing_crossings' sheet is read if available and passed to MaakKubusData in tbl_maken.R.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Github\GGData_tabellenboek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f314996661bdda06/Documenten/GitHub/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17B1887-B183-4C10-96A4-B1DE6FF4E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{A17B1887-B183-4C10-96A4-B1DE6FF4E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69235877-BA40-4754-B976-57553F3C4C7B}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="731" firstSheet="4" activeTab="13" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="731" firstSheet="4" activeTab="15" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="opmaak" sheetId="6" r:id="rId13"/>
     <sheet name="swing_configuraties" sheetId="20" r:id="rId14"/>
     <sheet name="swing_variabelen" sheetId="18" r:id="rId15"/>
+    <sheet name="swing_crossings" sheetId="21" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1720,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3ECE10-9C11-42F2-BAC4-98A7CB15471E}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="I20:J20"/>
     </sheetView>
   </sheetViews>
@@ -1848,10 +1849,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE8AA37-4D9A-4ED0-A142-2CF818365C43}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,88 +1860,82 @@
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>183</v>
       </c>
-      <c r="B1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -1958,6 +1953,31 @@
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE4C7B0-38B4-45EA-84A8-834557EF5F11}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature: Add weegfactor per variable in MakeKubus
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f314996661bdda06/Documenten/GitHub/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{A17B1887-B183-4C10-96A4-B1DE6FF4E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69235877-BA40-4754-B976-57553F3C4C7B}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{A17B1887-B183-4C10-96A4-B1DE6FF4E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8F8BB5E-A84B-44C9-9D8D-1C031B4F38AB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="731" firstSheet="4" activeTab="15" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="731" firstSheet="4" activeTab="14" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="211">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -1849,93 +1849,100 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE8AA37-4D9A-4ED0-A142-2CF818365C43}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -1964,7 +1971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE4C7B0-38B4-45EA-84A8-834557EF5F11}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -2267,7 +2274,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
afkapwaarde (was missing_voor_privacy) uit configuratiebestand halen als deze aanwezig is
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f314996661bdda06/Documenten/GitHub/GGData_tabellenboek/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Github\GGData_tabellenboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{A17B1887-B183-4C10-96A4-B1DE6FF4E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8F8BB5E-A84B-44C9-9D8D-1C031B4F38AB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC06673E-B887-4E2E-9AFD-ECA14BD84156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="731" firstSheet="4" activeTab="14" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15345" tabRatio="731" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="212">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -684,6 +684,9 @@
   </si>
   <si>
     <t>gemeentecode_regio</t>
+  </si>
+  <si>
+    <t>swing_afkapwaarde</t>
   </si>
 </sst>
 </file>
@@ -1054,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1077,7 @@
     <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1135,8 +1138,11 @@
       <c r="T1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1196,6 +1202,9 @@
       </c>
       <c r="T2" t="s">
         <v>173</v>
+      </c>
+      <c r="U2">
+        <v>-99996</v>
       </c>
     </row>
   </sheetData>
@@ -1851,7 +1860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE8AA37-4D9A-4ED0-A142-2CF818365C43}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>

</xml_diff>